<commit_message>
Fixed exporting tests for yss account reports
Former-commit-id: 4269109008c55df74b7fe4abf8ccd14fab94f560
</commit_message>
<xml_diff>
--- a/tests/resources/repo_yss_account_report.xlsx
+++ b/tests/resources/repo_yss_account_report.xlsx
@@ -51,7 +51,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" s="0" t="inlineStr">
         <is>
           <t>accountName</t>
@@ -157,539 +157,681 @@
           <t>valuePerAllConv</t>
         </is>
       </c>
+      <c r="V1" s="0" t="inlineStr">
+        <is>
+          <t>accountid</t>
+        </is>
+      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>DgAVzE2lec</t>
+          <t>C3sFHc9Txk</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>431,626</t>
+          <t>1,584,598</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>1,760,300</t>
+          <t>6,604,331</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>4,048,933</t>
+          <t>13,962,080</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>20,135.71</t>
+          <t>21,156.94</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>37,298,042</t>
+          <t>141,605,592</t>
         </is>
       </c>
       <c r="G2" s="0" t="inlineStr">
         <is>
-          <t>21,296.83</t>
+          <t>21,087.74</t>
         </is>
       </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
-          <t>20,673.90</t>
+          <t>20,590.70</t>
         </is>
       </c>
       <c r="I2" s="0" t="inlineStr">
         <is>
-          <t>21,029.93</t>
+          <t>20,598.08</t>
         </is>
       </c>
       <c r="J2" s="0" t="inlineStr">
         <is>
-          <t>20,027.82</t>
+          <t>20,701.05</t>
         </is>
       </c>
       <c r="K2" s="0" t="inlineStr">
         <is>
-          <t>20,726.76</t>
+          <t>21,098.50</t>
         </is>
       </c>
       <c r="L2" s="0" t="inlineStr">
         <is>
-          <t>19,847.93</t>
+          <t>20,950.55</t>
         </is>
       </c>
       <c r="M2" s="0" t="inlineStr">
         <is>
-          <t>21,281.37</t>
+          <t>20,960.78</t>
         </is>
       </c>
       <c r="N2" s="0" t="inlineStr">
         <is>
-          <t>20,832.80</t>
+          <t>20,764.06</t>
         </is>
       </c>
       <c r="O2" s="0" t="inlineStr">
         <is>
-          <t>21,358.70</t>
+          <t>21,153.01</t>
         </is>
       </c>
       <c r="P2" s="0" t="inlineStr">
         <is>
-          <t>21,443.72</t>
+          <t>20,750.28</t>
         </is>
       </c>
       <c r="Q2" s="0" t="inlineStr">
         <is>
-          <t>18,273,642.22</t>
+          <t>65,418,560.96</t>
         </is>
       </c>
       <c r="R2" s="0" t="inlineStr">
         <is>
-          <t>20,327.36</t>
+          <t>20,880.43</t>
         </is>
       </c>
       <c r="S2" s="0" t="inlineStr">
         <is>
-          <t>17,453,639.61</t>
+          <t>66,483,063.26</t>
         </is>
       </c>
       <c r="T2" s="0" t="inlineStr">
         <is>
-          <t>20,575.30</t>
+          <t>20,741.32</t>
         </is>
       </c>
       <c r="U2" s="0" t="inlineStr">
         <is>
-          <t>21,025.52</t>
+          <t>21,285.33</t>
+        </is>
+      </c>
+      <c r="V2" s="0" t="inlineStr">
+        <is>
+          <t>70,795</t>
         </is>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>SAdqHlv98A</t>
+          <t>SoTVSVuH0w</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>429,595</t>
+          <t>1,584,598</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>1,677,304</t>
+          <t>6,604,331</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>3,870,431</t>
+          <t>13,962,080</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>20,894.72</t>
+          <t>21,156.94</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>38,512,155</t>
+          <t>141,605,592</t>
         </is>
       </c>
       <c r="G3" s="0" t="inlineStr">
         <is>
-          <t>20,594.69</t>
+          <t>21,087.74</t>
         </is>
       </c>
       <c r="H3" s="0" t="inlineStr">
         <is>
-          <t>20,885.30</t>
+          <t>20,590.70</t>
         </is>
       </c>
       <c r="I3" s="0" t="inlineStr">
         <is>
-          <t>21,392.93</t>
+          <t>20,598.08</t>
         </is>
       </c>
       <c r="J3" s="0" t="inlineStr">
         <is>
-          <t>21,125.43</t>
+          <t>20,701.05</t>
         </is>
       </c>
       <c r="K3" s="0" t="inlineStr">
         <is>
-          <t>20,184.24</t>
+          <t>21,098.50</t>
         </is>
       </c>
       <c r="L3" s="0" t="inlineStr">
         <is>
-          <t>20,494.48</t>
+          <t>20,950.55</t>
         </is>
       </c>
       <c r="M3" s="0" t="inlineStr">
         <is>
-          <t>20,526.96</t>
+          <t>20,960.78</t>
         </is>
       </c>
       <c r="N3" s="0" t="inlineStr">
         <is>
-          <t>20,707.31</t>
+          <t>20,764.06</t>
         </is>
       </c>
       <c r="O3" s="0" t="inlineStr">
         <is>
-          <t>20,234.70</t>
+          <t>21,153.01</t>
         </is>
       </c>
       <c r="P3" s="0" t="inlineStr">
         <is>
-          <t>20,878.45</t>
+          <t>20,750.28</t>
         </is>
       </c>
       <c r="Q3" s="0" t="inlineStr">
         <is>
-          <t>17,967,926.51</t>
+          <t>65,418,560.96</t>
         </is>
       </c>
       <c r="R3" s="0" t="inlineStr">
         <is>
-          <t>20,427.02</t>
+          <t>20,880.43</t>
         </is>
       </c>
       <c r="S3" s="0" t="inlineStr">
         <is>
-          <t>17,348,981.99</t>
+          <t>66,483,063.26</t>
         </is>
       </c>
       <c r="T3" s="0" t="inlineStr">
         <is>
-          <t>20,557.94</t>
+          <t>20,741.32</t>
         </is>
       </c>
       <c r="U3" s="0" t="inlineStr">
         <is>
-          <t>21,118.23</t>
+          <t>21,285.33</t>
+        </is>
+      </c>
+      <c r="V3" s="0" t="inlineStr">
+        <is>
+          <t>70,795</t>
         </is>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>sTaagkkYwn</t>
+          <t>aqZaakvSNq</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>355,986</t>
+          <t>1,584,598</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>1,505,129</t>
+          <t>6,604,331</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>3,213,778</t>
+          <t>13,962,080</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>20,130.81</t>
+          <t>21,156.94</t>
         </is>
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>31,534,678</t>
+          <t>141,605,592</t>
         </is>
       </c>
       <c r="G4" s="0" t="inlineStr">
         <is>
-          <t>21,635.83</t>
+          <t>21,087.74</t>
         </is>
       </c>
       <c r="H4" s="0" t="inlineStr">
         <is>
-          <t>20,682.64</t>
+          <t>20,590.70</t>
         </is>
       </c>
       <c r="I4" s="0" t="inlineStr">
         <is>
-          <t>20,091.19</t>
+          <t>20,598.08</t>
         </is>
       </c>
       <c r="J4" s="0" t="inlineStr">
         <is>
-          <t>20,515.58</t>
+          <t>20,701.05</t>
         </is>
       </c>
       <c r="K4" s="0" t="inlineStr">
         <is>
-          <t>20,669.81</t>
+          <t>21,098.50</t>
         </is>
       </c>
       <c r="L4" s="0" t="inlineStr">
         <is>
-          <t>20,599.66</t>
+          <t>20,950.55</t>
         </is>
       </c>
       <c r="M4" s="0" t="inlineStr">
         <is>
-          <t>20,884.20</t>
+          <t>20,960.78</t>
         </is>
       </c>
       <c r="N4" s="0" t="inlineStr">
         <is>
-          <t>20,587.60</t>
+          <t>20,764.06</t>
         </is>
       </c>
       <c r="O4" s="0" t="inlineStr">
         <is>
-          <t>19,985.88</t>
+          <t>21,153.01</t>
         </is>
       </c>
       <c r="P4" s="0" t="inlineStr">
         <is>
-          <t>19,819.64</t>
+          <t>20,750.28</t>
         </is>
       </c>
       <c r="Q4" s="0" t="inlineStr">
         <is>
-          <t>14,961,244.20</t>
+          <t>65,418,560.96</t>
         </is>
       </c>
       <c r="R4" s="0" t="inlineStr">
         <is>
-          <t>20,611.37</t>
+          <t>20,880.43</t>
         </is>
       </c>
       <c r="S4" s="0" t="inlineStr">
         <is>
-          <t>14,632,965.74</t>
+          <t>66,483,063.26</t>
         </is>
       </c>
       <c r="T4" s="0" t="inlineStr">
         <is>
-          <t>20,100.08</t>
+          <t>20,741.32</t>
         </is>
       </c>
       <c r="U4" s="0" t="inlineStr">
         <is>
-          <t>21,628.33</t>
+          <t>21,285.33</t>
+        </is>
+      </c>
+      <c r="V4" s="0" t="inlineStr">
+        <is>
+          <t>70,795</t>
         </is>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>n4ZDkajrir</t>
+          <t>imbbyolD4T</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>358,803</t>
+          <t>1,584,598</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>1,497,190</t>
+          <t>6,604,331</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>3,260,807</t>
+          <t>13,962,080</t>
         </is>
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>21,271.01</t>
+          <t>21,156.94</t>
         </is>
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
-          <t>31,061,346</t>
+          <t>141,605,592</t>
         </is>
       </c>
       <c r="G5" s="0" t="inlineStr">
         <is>
-          <t>20,219.04</t>
+          <t>21,087.74</t>
         </is>
       </c>
       <c r="H5" s="0" t="inlineStr">
         <is>
-          <t>20,786.91</t>
+          <t>20,590.70</t>
         </is>
       </c>
       <c r="I5" s="0" t="inlineStr">
         <is>
-          <t>21,038.66</t>
+          <t>20,598.08</t>
         </is>
       </c>
       <c r="J5" s="0" t="inlineStr">
         <is>
-          <t>20,738.54</t>
+          <t>20,701.05</t>
         </is>
       </c>
       <c r="K5" s="0" t="inlineStr">
         <is>
-          <t>20,718.03</t>
+          <t>21,098.50</t>
         </is>
       </c>
       <c r="L5" s="0" t="inlineStr">
         <is>
-          <t>21,100.88</t>
+          <t>20,950.55</t>
         </is>
       </c>
       <c r="M5" s="0" t="inlineStr">
         <is>
-          <t>21,038.69</t>
+          <t>20,960.78</t>
         </is>
       </c>
       <c r="N5" s="0" t="inlineStr">
         <is>
-          <t>20,865.08</t>
+          <t>20,764.06</t>
         </is>
       </c>
       <c r="O5" s="0" t="inlineStr">
         <is>
-          <t>20,691.46</t>
+          <t>21,153.01</t>
         </is>
       </c>
       <c r="P5" s="0" t="inlineStr">
         <is>
-          <t>20,969.71</t>
+          <t>20,750.28</t>
         </is>
       </c>
       <c r="Q5" s="0" t="inlineStr">
         <is>
-          <t>14,612,479.28</t>
+          <t>65,418,560.96</t>
         </is>
       </c>
       <c r="R5" s="0" t="inlineStr">
         <is>
-          <t>21,039.55</t>
+          <t>20,880.43</t>
         </is>
       </c>
       <c r="S5" s="0" t="inlineStr">
         <is>
-          <t>14,807,453.58</t>
+          <t>66,483,063.26</t>
         </is>
       </c>
       <c r="T5" s="0" t="inlineStr">
         <is>
-          <t>20,746.83</t>
+          <t>20,741.32</t>
         </is>
       </c>
       <c r="U5" s="0" t="inlineStr">
         <is>
-          <t>20,629.82</t>
+          <t>21,285.33</t>
+        </is>
+      </c>
+      <c r="V5" s="0" t="inlineStr">
+        <is>
+          <t>70,795</t>
         </is>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>olbZQGLxK2</t>
+          <t>OEXiADPjQd</t>
         </is>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>364,038</t>
+          <t>804,765</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>1,479,379</t>
+          <t>3,365,646</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>3,221,632</t>
+          <t>7,464,471</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>20,837.32</t>
+          <t>20,516.57</t>
         </is>
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
-          <t>33,160,068</t>
+          <t>73,586,762</t>
         </is>
       </c>
       <c r="G6" s="0" t="inlineStr">
         <is>
-          <t>21,336.05</t>
+          <t>21,136.75</t>
         </is>
       </c>
       <c r="H6" s="0" t="inlineStr">
         <is>
-          <t>21,513.25</t>
+          <t>20,643.88</t>
         </is>
       </c>
       <c r="I6" s="0" t="inlineStr">
         <is>
-          <t>20,876.77</t>
+          <t>21,130.84</t>
         </is>
       </c>
       <c r="J6" s="0" t="inlineStr">
         <is>
-          <t>21,184.91</t>
+          <t>21,024.48</t>
         </is>
       </c>
       <c r="K6" s="0" t="inlineStr">
         <is>
-          <t>21,830.71</t>
+          <t>20,864.22</t>
         </is>
       </c>
       <c r="L6" s="0" t="inlineStr">
         <is>
-          <t>21,130.15</t>
+          <t>21,263.28</t>
         </is>
       </c>
       <c r="M6" s="0" t="inlineStr">
         <is>
-          <t>20,871.48</t>
+          <t>20,890.87</t>
         </is>
       </c>
       <c r="N6" s="0" t="inlineStr">
         <is>
-          <t>21,573.64</t>
+          <t>20,539.14</t>
         </is>
       </c>
       <c r="O6" s="0" t="inlineStr">
         <is>
-          <t>21,096.28</t>
+          <t>20,816.25</t>
         </is>
       </c>
       <c r="P6" s="0" t="inlineStr">
         <is>
-          <t>21,134.36</t>
+          <t>20,560.25</t>
         </is>
       </c>
       <c r="Q6" s="0" t="inlineStr">
         <is>
-          <t>15,517,264.44</t>
+          <t>34,263,346.94</t>
         </is>
       </c>
       <c r="R6" s="0" t="inlineStr">
         <is>
-          <t>20,934.78</t>
+          <t>20,951.21</t>
         </is>
       </c>
       <c r="S6" s="0" t="inlineStr">
         <is>
-          <t>14,813,139.32</t>
+          <t>33,334,928.96</t>
         </is>
       </c>
       <c r="T6" s="0" t="inlineStr">
         <is>
-          <t>21,761.96</t>
+          <t>21,126.07</t>
         </is>
       </c>
       <c r="U6" s="0" t="inlineStr">
         <is>
-          <t>21,181.52</t>
+          <t>20,480.14</t>
+        </is>
+      </c>
+      <c r="V6" s="0" t="inlineStr">
+        <is>
+          <t>18,734</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>0WSSd6geVU</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>804,765</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>3,365,646</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>7,464,471</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>20,516.57</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>73,586,762</t>
+        </is>
+      </c>
+      <c r="G7" s="0" t="inlineStr">
+        <is>
+          <t>21,136.75</t>
+        </is>
+      </c>
+      <c r="H7" s="0" t="inlineStr">
+        <is>
+          <t>20,643.88</t>
+        </is>
+      </c>
+      <c r="I7" s="0" t="inlineStr">
+        <is>
+          <t>21,130.84</t>
+        </is>
+      </c>
+      <c r="J7" s="0" t="inlineStr">
+        <is>
+          <t>21,024.48</t>
+        </is>
+      </c>
+      <c r="K7" s="0" t="inlineStr">
+        <is>
+          <t>20,864.22</t>
+        </is>
+      </c>
+      <c r="L7" s="0" t="inlineStr">
+        <is>
+          <t>21,263.28</t>
+        </is>
+      </c>
+      <c r="M7" s="0" t="inlineStr">
+        <is>
+          <t>20,890.87</t>
+        </is>
+      </c>
+      <c r="N7" s="0" t="inlineStr">
+        <is>
+          <t>20,539.14</t>
+        </is>
+      </c>
+      <c r="O7" s="0" t="inlineStr">
+        <is>
+          <t>20,816.25</t>
+        </is>
+      </c>
+      <c r="P7" s="0" t="inlineStr">
+        <is>
+          <t>20,560.25</t>
+        </is>
+      </c>
+      <c r="Q7" s="0" t="inlineStr">
+        <is>
+          <t>34,263,346.94</t>
+        </is>
+      </c>
+      <c r="R7" s="0" t="inlineStr">
+        <is>
+          <t>20,951.21</t>
+        </is>
+      </c>
+      <c r="S7" s="0" t="inlineStr">
+        <is>
+          <t>33,334,928.96</t>
+        </is>
+      </c>
+      <c r="T7" s="0" t="inlineStr">
+        <is>
+          <t>21,126.07</t>
+        </is>
+      </c>
+      <c r="U7" s="0" t="inlineStr">
+        <is>
+          <t>20,480.14</t>
+        </is>
+      </c>
+      <c r="V7" s="0" t="inlineStr">
+        <is>
+          <t>18,734</t>
         </is>
       </c>
     </row>

</xml_diff>